<commit_message>
xls2xml - bugfix box: categories
categories are made of Studio->Series->Season
</commit_message>
<xml_diff>
--- a/xls2xml/tests_box/input_box_last_version.xlsx
+++ b/xls2xml/tests_box/input_box_last_version.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="538">
   <si>
     <t xml:space="preserve">uuid_box</t>
   </si>
@@ -1556,6 +1556,15 @@
   </si>
   <si>
     <t xml:space="preserve">por:Faroeste|eng:Western</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63f6fc27-d1e6-41b4-bc55-a045ed95609f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">por:Inverleigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studio</t>
   </si>
   <si>
     <t xml:space="preserve">title</t>
@@ -2059,10 +2068,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="R6" activeCellId="1" sqref="B:B R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12301,10 +12310,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12866,6 +12875,32 @@
         <v>467</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="D22" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>467</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -12882,43 +12917,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="40.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="41.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="226.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="39.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="41.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="16" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="16" width="41.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="226.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="39.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="41.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="16" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
         <v>457</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>510</v>
-      </c>
-      <c r="G1" s="20"/>
+        <v>512</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>513</v>
+      </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
@@ -12927,125 +12964,141 @@
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>511</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>512</v>
+        <v>514</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="E2" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>515</v>
+        <v>516</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="F2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>517</v>
+        <v>519</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>521</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="F3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>518</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>519</v>
-      </c>
-      <c r="E3" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>520</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>521</v>
+        <v>523</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>523</v>
-      </c>
-      <c r="E4" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>515</v>
+        <v>525</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="F4" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>524</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>525</v>
+        <v>527</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>527</v>
-      </c>
-      <c r="E5" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>515</v>
+        <v>529</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="F5" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>528</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>529</v>
+        <v>531</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>531</v>
-      </c>
-      <c r="E6" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>533</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="F6" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>532</v>
-      </c>
-      <c r="B7" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>475</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>533</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>534</v>
-      </c>
-      <c r="E7" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>515</v>
+      <c r="D7" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="F7" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>